<commit_message>
Implentation of angle calculations - BAD - leads to convergance to zero or bigger angles
</commit_message>
<xml_diff>
--- a/Angles.xlsx
+++ b/Angles.xlsx
@@ -9,14 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="3080" windowWidth="15420" windowHeight="13860" xr2:uid="{7929ADFC-B732-484D-AE82-60DEDA38B34C}"/>
+    <workbookView xWindow="13380" yWindow="3080" windowWidth="15420" windowHeight="13860" activeTab="1" xr2:uid="{7929ADFC-B732-484D-AE82-60DEDA38B34C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
+    <sheet name="Constant X" sheetId="1" r:id="rId1"/>
+    <sheet name="Constant Speed" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="X">Blatt1!$B$3</definedName>
-    <definedName name="Y">Blatt1!$B$2</definedName>
+    <definedName name="X" localSheetId="1">'Constant Speed'!$B$4</definedName>
+    <definedName name="X">'Constant X'!$B$4</definedName>
+    <definedName name="Y" localSheetId="1">'Constant Speed'!$B$3</definedName>
+    <definedName name="Y">'Constant X'!$B$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Y</t>
   </si>
@@ -55,13 +58,32 @@
   </si>
   <si>
     <t>alpha Grad</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>Initial Speed</t>
+  </si>
+  <si>
+    <t>New Alpha</t>
+  </si>
+  <si>
+    <t>New X</t>
+  </si>
+  <si>
+    <t>New Speed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00&quot;°&quot;"/>
   </numFmts>
   <fonts count="2">
@@ -95,17 +117,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+  <cellStyles count="3">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BF40FE-7E85-BD4B-84D0-627187E6D1CD}">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -430,80 +455,402 @@
     <col min="2" max="2" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>-2</v>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <f>SQRT(4+4)</f>
+        <v>2.8284271247461903</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <f>Y</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f>SQRT(ABS(B1^2-C3^2))</f>
+        <v>2.0000000000000004</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <f>Y/X</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <f>ATAN(Y/X)</f>
-        <v>-0.78539816339744828</v>
-      </c>
-      <c r="C6" s="1">
-        <f>DEGREES(B6)</f>
-        <v>-45</v>
+        <f>SQRT(Y^2+X^2)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="C5">
+        <f>SQRT(C3^2+C4^2)</f>
+        <v>2.8284271247461903</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <f>Y/X</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <f>ATAN(Y/X)</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C8" s="1">
+        <f>DEGREES(B8)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
+      <c r="B9">
+        <f>TAN(B8)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <f>TAN(B8)*X</f>
+        <v>1.9999999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14">
+        <f>SIGN(Y)</f>
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f>SIGN(Y)</f>
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>SIGN(Y)</f>
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f>SIGN(Y)</f>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f>SIGN(Y)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
+        <f>-100%*B14</f>
+        <v>-1</v>
+      </c>
+      <c r="C15" s="2">
+        <f>-50%*C14</f>
+        <v>-0.5</v>
+      </c>
+      <c r="D15" s="2">
+        <f>0%*D14</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <f>50%*E14</f>
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="2">
+        <f>100%*F14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <f>Y*(1+B15)</f>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f>Y*(1+C15)</f>
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f>Y*(1+D15)</f>
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <f>Y*(1+E15)</f>
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <f>Y*(1+F15)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <f>ATAN(B16/X)</f>
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f>ATAN(C16/X)</f>
+        <v>0.46364760900080609</v>
+      </c>
+      <c r="D17">
+        <f>ATAN(D16/X)</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="E17">
+        <f>ATAN(E16/X)</f>
+        <v>0.98279372324732905</v>
+      </c>
+      <c r="F17">
+        <f>ATAN(F16/X)</f>
+        <v>1.1071487177940904</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" ref="B18:E18" si="0">DEGREES(B17)</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>26.56505117707799</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>56.309932474020215</v>
+      </c>
+      <c r="F18" s="1">
+        <f>DEGREES(F17)</f>
+        <v>63.43494882292201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6631C8-31DC-8C44-8EBE-83610FEE632E}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <f>SQRT(4+4)</f>
+        <v>2.8284271247461903</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f>Y</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f>SQRT(ABS(B1^2-C3^2))</f>
+        <v>2.8284271247461898</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <f>SQRT(Y^2+X^2)</f>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="C5">
+        <f>SQRT(C3^2+C4^2)</f>
+        <v>4.8989794855663558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
       <c r="B7">
-        <f>TAN(B6)</f>
-        <v>-0.99999999999999989</v>
+        <f>ATAN(Y/X)</f>
+        <v>1.1071487177940904</v>
+      </c>
+      <c r="C7" s="1">
+        <f>DEGREES(B7)</f>
+        <v>63.43494882292201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <f>TAN(B7)</f>
+        <v>1.9999999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="B10">
+        <f>SIGN(Y)</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>SIGN(Y)</f>
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f>SIGN(Y)</f>
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f>SIGN(Y)</f>
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f>SIGN(Y)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <f>-100%*B10</f>
+        <v>-1</v>
+      </c>
+      <c r="C11" s="2">
+        <f>-50%*C10</f>
+        <v>-0.5</v>
+      </c>
+      <c r="D11" s="2">
+        <f>0%*D10</f>
         <v>0</v>
       </c>
-      <c r="B10">
-        <f>TAN(B6)*X</f>
-        <v>-1.9999999999999998</v>
+      <c r="E11" s="2">
+        <f>50%*E10</f>
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="2">
+        <f>100%*F10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3">
+        <f>$B$7*(1+(B11/3))</f>
+        <v>0.73809914519606035</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ref="C12:F12" si="0">$B$7*(1+(C11/3))</f>
+        <v>0.92262393149507538</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1071487177940904</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2916735040931056</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4761982903921205</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="2">
-        <v>-1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>-0.5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B13" s="1">
+        <f>DEGREES(B12)</f>
+        <v>42.289965881948007</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" ref="C13:F13" si="1">DEGREES(C12)</f>
+        <v>52.862457352435008</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>63.43494882292201</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>74.007440293409019</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>84.579931763895999</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -511,74 +858,74 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <f>Y*(1+B13)</f>
-        <v>0</v>
+        <f>$B$1*SIN(B12)</f>
+        <v>1.9032004519946746</v>
       </c>
       <c r="C14">
-        <f>Y*(1+C13)</f>
-        <v>-1</v>
+        <f t="shared" ref="C14:F14" si="2">$B$1*SIN(C12)</f>
+        <v>2.254789605044818</v>
       </c>
       <c r="D14">
-        <f>Y*(1+D13)</f>
-        <v>-2</v>
+        <f t="shared" si="2"/>
+        <v>2.5298221281347035</v>
       </c>
       <c r="E14">
-        <f>Y*(1+E13)</f>
-        <v>-3</v>
+        <f t="shared" si="2"/>
+        <v>2.7189598714652918</v>
       </c>
       <c r="F14">
-        <f>Y*(1+F13)</f>
-        <v>-4</v>
+        <f t="shared" si="2"/>
+        <v>2.8157810614949259</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <f>ATAN(B14/X)</f>
-        <v>0</v>
+        <f>$B$1*COS(B12)</f>
+        <v>2.0923259878726514</v>
       </c>
       <c r="C15">
-        <f>ATAN(C14/X)</f>
-        <v>-0.46364760900080609</v>
+        <f t="shared" ref="C15:F15" si="3">$B$1*COS(C12)</f>
+        <v>1.7076076355480014</v>
       </c>
       <c r="D15">
-        <f>ATAN(D14/X)</f>
-        <v>-0.78539816339744828</v>
+        <f t="shared" si="3"/>
+        <v>1.2649110640673522</v>
       </c>
       <c r="E15">
-        <f>ATAN(E14/X)</f>
-        <v>-0.98279372324732905</v>
+        <f t="shared" si="3"/>
+        <v>0.77926710270705357</v>
       </c>
       <c r="F15">
-        <f>ATAN(F14/X)</f>
-        <v>-1.1071487177940904</v>
+        <f t="shared" si="3"/>
+        <v>0.26716476887214946</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1">
-        <f t="shared" ref="B16:E16" si="0">DEGREES(B15)</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <f t="shared" si="0"/>
-        <v>-26.56505117707799</v>
-      </c>
-      <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>-45</v>
-      </c>
-      <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>-56.309932474020215</v>
-      </c>
-      <c r="F16" s="1">
-        <f>DEGREES(F15)</f>
-        <v>-63.43494882292201</v>
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f>SQRT(B14^2+B15^2)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:F16" si="4">SQRT(C14^2+C15^2)</f>
+        <v>2.8284271247461907</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="4"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>2.8284271247461903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>